<commit_message>
_data_analysis 폴더 추가 / data,web 구분
</commit_message>
<xml_diff>
--- a/_documents/요구사항정의서(KPC-STS-SRS01).xlsx
+++ b/_documents/요구사항정의서(KPC-STS-SRS01).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\스프린트 II\_documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sky_to_Solar\_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8925"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8925" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="표지" sheetId="7" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
   <si>
     <t>비고</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -187,33 +187,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>메인 홈페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>푸터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-002-02</t>
+  </si>
+  <si>
     <t>비기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>메인 홈페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>푸터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-002-02</t>
-  </si>
-  <si>
-    <t>비기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>결과 페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -229,67 +225,7 @@
     <t>REQ-SFR-003-02</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>○</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">시작하기 버튼
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>•</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 버튼을 누르면 REQ-SFR-002 로 이동</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>REQ-SFR-002-03</t>
-  </si>
-  <si>
-    <t>업로드 할 수 있는 사진 기준 예시를 보여준다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>○ 사진 업로드 
@@ -298,458 +234,585 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>○</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">결과 보여주기
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">태양광 에너지 수치
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>생산되는 에너지 양으로 할 수 있는 일 보여주기</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-001-02</t>
+  </si>
+  <si>
+    <t>헤더</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-005</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">○ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">다시 시작 버튼
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>누르면 업로드 페이지로 이동</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">○ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">로고
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>로고 누르면 REQ-SFR-001 로 이동</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>○</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 우측 상단 메뉴
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">REQ-SFR-001 의 섹션 별 이동
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>REQ-SFR-001 로 이동</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-004-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-004-02</t>
+  </si>
+  <si>
+    <t>비기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>○</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">팀 프로젝트 깃허브 주소 
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>주소 클릭 시 해당 깃허브로 이동</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-005-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-005-02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-006-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-003-03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-003-03, REQ-SFR-004, REQ-SFR-005, REQ-SFR-006 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강다솜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강다솜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-002-01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-006-02</t>
+  </si>
+  <si>
+    <t>REQ-SFR-002-01에 모델 연동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반복 학습을 통해 모델 완성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학습 데이터 수집 후 테스트 진행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-006-03</t>
+  </si>
+  <si>
+    <t>KepcoA 스프린트II 프로젝트 Team Sunrise (1조)</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">  KepcoA Sprint II Project Team Sunrise</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>○</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">시작하기 버튼
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 버튼을 누르면 REQ-SFR-002 로 이동</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">○ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">가장 상단에 프로젝트 간단 소개 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">○ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">프로젝트 관련 내용 섹션 별 구분
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>• 스크롤로 내릴 수 있게 한다</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>○ 유의사항
+   • 업로드 할 수 있는 사진 기준 예시를 보여준다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>○ 사진 변경 사이트 이동 버튼
    • 사진을 어안렌즈 필터로 변경가능한 사이트 링크</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>○</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">결과 보여주기
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>•</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">태양광 에너지 수치
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>•</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>생산되는 에너지 양으로 할 수 있는 일 보여주기</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-001-02</t>
-  </si>
-  <si>
-    <t>헤더</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-005</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">○ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">다시 시작 버튼
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>누르면 업로드 페이지로 이동</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">○ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">로고
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>로고 누르면 REQ-SFR-001 로 이동</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>○</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 우측 상단 메뉴
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">REQ-SFR-001 의 섹션 별 이동
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>REQ-SFR-001 로 이동</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가장 상단에 프로젝트 설명 노출</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-004-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-004-02</t>
-  </si>
-  <si>
-    <t>비기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>팀원들 깃허브 아이디 나열</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>○</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.35"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">팀 프로젝트 깃허브 주소 
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>주소 클릭 시 해당 깃허브로 이동</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-005-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-005-02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-006-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-003-03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-003-03, REQ-SFR-004, REQ-SFR-005, REQ-SFR-006 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-002-01 상세 요구사항 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강다솜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강다솜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-002-01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>딥러닝 모델 웹 연결</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-006-02</t>
-  </si>
-  <si>
-    <t>REQ-SFR-002-01에 모델 연동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>반복 학습을 통해 모델 완성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>학습 데이터 수집 후 테스트 진행</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQ-SFR-006-03</t>
-  </si>
-  <si>
-    <t>KepcoA 스프린트II 프로젝트 Team Sunrise (1조)</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">  KepcoA Sprint II Project Team Sunrise</t>
-    </r>
+    <t>기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀원 깃허브 아이디 나열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>딥러닝 모델</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REQ-SFR-002-01 상세 요구사항 수정 (드래그 앤 드롭 기능)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kaggle Dataset 이용 :
+https://www.kaggle.com/datasets/maksboralessa/solar-energy-forecasting-using-low-res-sky-images</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1169,7 +1232,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1326,6 +1389,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1344,6 +1413,9 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1354,13 +1426,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1386,23 +1467,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2145,7 +2211,7 @@
   </sheetPr>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
@@ -2200,10 +2266,10 @@
       <c r="J3" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="52"/>
+      <c r="L3" s="54"/>
       <c r="M3" s="44"/>
     </row>
     <row r="4" spans="1:13" ht="21" customHeight="1">
@@ -2275,10 +2341,10 @@
       <c r="F8" s="45"/>
       <c r="G8" s="45"/>
       <c r="H8" s="45"/>
-      <c r="I8" s="76" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8" s="75"/>
+      <c r="I8" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="52"/>
       <c r="K8" s="45"/>
       <c r="L8" s="45"/>
       <c r="M8" s="44"/>
@@ -2315,79 +2381,79 @@
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1">
       <c r="A11" s="46"/>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
       <c r="M11" s="44"/>
     </row>
     <row r="12" spans="1:13" ht="21" customHeight="1">
       <c r="A12" s="46"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
       <c r="M12" s="44"/>
     </row>
     <row r="13" spans="1:13" ht="21" customHeight="1">
       <c r="A13" s="46"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
       <c r="M13" s="44"/>
     </row>
     <row r="14" spans="1:13" ht="21" customHeight="1">
       <c r="A14" s="46"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
       <c r="M14" s="44"/>
     </row>
     <row r="15" spans="1:13" ht="21" customHeight="1" thickBot="1">
       <c r="A15" s="46"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
       <c r="M15" s="44"/>
     </row>
     <row r="16" spans="1:13" ht="21" customHeight="1" thickTop="1">
@@ -2455,13 +2521,13 @@
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
-      <c r="E20" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
+      <c r="E20" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
       <c r="J20" s="45"/>
       <c r="K20" s="45"/>
       <c r="L20" s="45"/>
@@ -2472,11 +2538,11 @@
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
       <c r="D21" s="45"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="77"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
       <c r="J21" s="45"/>
       <c r="K21" s="45"/>
       <c r="L21" s="45"/>
@@ -2488,11 +2554,11 @@
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
-      <c r="F22" s="56">
+      <c r="F22" s="58">
         <v>45309</v>
       </c>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
       <c r="I22" s="45"/>
       <c r="J22" s="45"/>
       <c r="K22" s="45"/>
@@ -2505,9 +2571,9 @@
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
       <c r="I23" s="45"/>
       <c r="J23" s="45"/>
       <c r="K23" s="45"/>
@@ -2630,7 +2696,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F10" sqref="F10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="16.5"/>
@@ -2662,7 +2728,7 @@
     <row r="2" spans="1:13" ht="21" customHeight="1">
       <c r="A2" s="22"/>
       <c r="B2" s="32" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="20"/>
@@ -2672,11 +2738,11 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
       <c r="J2" s="20"/>
-      <c r="K2" s="58" t="str">
+      <c r="K2" s="61" t="str">
         <f>표지!B11</f>
         <v xml:space="preserve">요구사항 정의서 </v>
       </c>
-      <c r="L2" s="58"/>
+      <c r="L2" s="61"/>
       <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" ht="31.5">
@@ -2696,19 +2762,19 @@
     </row>
     <row r="4" spans="1:13" ht="21" customHeight="1">
       <c r="A4" s="22"/>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
       <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" ht="21" customHeight="1">
@@ -2734,17 +2800,17 @@
       <c r="C6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60" t="s">
+      <c r="E6" s="63"/>
+      <c r="F6" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
       <c r="K6" s="27" t="s">
         <v>16</v>
       </c>
@@ -2761,17 +2827,17 @@
       <c r="C7" s="24">
         <v>45309</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="74"/>
-      <c r="F7" s="61" t="s">
+      <c r="E7" s="65"/>
+      <c r="F7" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="62"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="68"/>
       <c r="K7" s="23" t="s">
         <v>22</v>
       </c>
@@ -2788,22 +2854,22 @@
       <c r="C8" s="24">
         <v>45310</v>
       </c>
-      <c r="D8" s="73" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="74"/>
-      <c r="F8" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="62"/>
+      <c r="D8" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="65"/>
+      <c r="F8" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="68"/>
       <c r="K8" s="23" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="M8" s="18"/>
     </row>
@@ -2811,15 +2877,15 @@
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="62"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="68"/>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="18"/>
@@ -2828,13 +2894,13 @@
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="62"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="68"/>
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="18"/>
@@ -2843,13 +2909,13 @@
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="62"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="68"/>
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="18"/>
@@ -2858,13 +2924,13 @@
       <c r="A12" s="22"/>
       <c r="B12" s="25"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="62"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="68"/>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
       <c r="M12" s="18"/>
@@ -2873,13 +2939,13 @@
       <c r="A13" s="22"/>
       <c r="B13" s="25"/>
       <c r="C13" s="26"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="62"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="68"/>
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
       <c r="M13" s="18"/>
@@ -2888,13 +2954,13 @@
       <c r="A14" s="22"/>
       <c r="B14" s="25"/>
       <c r="C14" s="26"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="62"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="68"/>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
       <c r="M14" s="18"/>
@@ -2903,13 +2969,13 @@
       <c r="A15" s="22"/>
       <c r="B15" s="25"/>
       <c r="C15" s="26"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="62"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="68"/>
       <c r="K15" s="25"/>
       <c r="L15" s="25"/>
       <c r="M15" s="18"/>
@@ -2918,13 +2984,13 @@
       <c r="A16" s="22"/>
       <c r="B16" s="25"/>
       <c r="C16" s="26"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="62"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="18"/>
@@ -2933,13 +2999,13 @@
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="62"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="68"/>
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="18"/>
@@ -2948,13 +3014,13 @@
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="62"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="68"/>
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
       <c r="M18" s="18"/>
@@ -2963,13 +3029,13 @@
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="62"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
       <c r="M19" s="18"/>
@@ -2978,13 +3044,13 @@
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="24"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="62"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="18"/>
@@ -2993,13 +3059,13 @@
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="62"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="68"/>
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="18"/>
@@ -3008,13 +3074,13 @@
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="24"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="62"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="68"/>
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="18"/>
@@ -3023,13 +3089,13 @@
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="24"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="62"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="68"/>
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="18"/>
@@ -3038,13 +3104,13 @@
       <c r="A24" s="22"/>
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="62"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="68"/>
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
       <c r="M24" s="18"/>
@@ -3181,8 +3247,8 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -3200,68 +3266,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="66" t="s">
+      <c r="I3" s="72" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="1:9" ht="33">
       <c r="A5" s="7">
@@ -3283,32 +3349,32 @@
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="49.5">
       <c r="A6" s="7">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -3324,16 +3390,16 @@
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -3355,35 +3421,35 @@
         <v>29</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="33">
       <c r="A9" s="7">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -3399,16 +3465,16 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G10" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -3424,16 +3490,16 @@
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -3449,16 +3515,16 @@
         <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -3474,16 +3540,16 @@
         <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -3499,16 +3565,16 @@
         <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -3524,16 +3590,16 @@
         <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -3543,27 +3609,27 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" ht="66">
       <c r="A17" s="7">
         <v>13</v>
       </c>
@@ -3574,19 +3640,21 @@
         <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="78" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7">
@@ -3599,16 +3667,16 @@
         <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -3621,19 +3689,19 @@
         <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>

</xml_diff>